<commit_message>
Updated 3 consecutive scores
</commit_message>
<xml_diff>
--- a/backend/data/odds/nfl odds 2021-22.xlsx
+++ b/backend/data/odds/nfl odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I241"/>
+  <dimension ref="A1:I243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8395,6 +8395,72 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Titans</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>49ers</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>155</v>
+      </c>
+      <c r="E242" t="n">
+        <v>-180</v>
+      </c>
+      <c r="F242" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G242" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="H242" t="n">
+        <v>16</v>
+      </c>
+      <c r="I242" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Packers</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Browns</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>-320</v>
+      </c>
+      <c r="E243" t="n">
+        <v>250</v>
+      </c>
+      <c r="F243" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="G243" t="n">
+        <v>46</v>
+      </c>
+      <c r="H243" t="n">
+        <v>16</v>
+      </c>
+      <c r="I243" t="n">
+        <v>2021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Super Bowl Week update
</commit_message>
<xml_diff>
--- a/backend/data/odds/nfl odds 2021-22.xlsx
+++ b/backend/data/odds/nfl odds 2021-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I279"/>
+  <dimension ref="A1:I286"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9466,16 +9466,16 @@
         </is>
       </c>
       <c r="D274" t="n">
-        <v>-225</v>
+        <v>-280</v>
       </c>
       <c r="E274" t="n">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="F274" t="n">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="G274" t="n">
-        <v>49</v>
+        <v>48.5</v>
       </c>
       <c r="H274" t="n">
         <v>19</v>
@@ -9499,16 +9499,16 @@
         </is>
       </c>
       <c r="D275" t="n">
-        <v>-200</v>
+        <v>-210</v>
       </c>
       <c r="E275" t="n">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="F275" t="n">
         <v>4</v>
       </c>
       <c r="G275" t="n">
-        <v>43.5</v>
+        <v>43</v>
       </c>
       <c r="H275" t="n">
         <v>19</v>
@@ -9532,16 +9532,16 @@
         </is>
       </c>
       <c r="D276" t="n">
-        <v>-400</v>
+        <v>-335</v>
       </c>
       <c r="E276" t="n">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="F276" t="n">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="G276" t="n">
-        <v>46</v>
+        <v>47.5</v>
       </c>
       <c r="H276" t="n">
         <v>19</v>
@@ -9565,16 +9565,16 @@
         </is>
       </c>
       <c r="D277" t="n">
-        <v>-165</v>
+        <v>-170</v>
       </c>
       <c r="E277" t="n">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F277" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G277" t="n">
-        <v>50.5</v>
+        <v>51</v>
       </c>
       <c r="H277" t="n">
         <v>19</v>
@@ -9598,16 +9598,16 @@
         </is>
       </c>
       <c r="D278" t="n">
-        <v>-675</v>
+        <v>-600</v>
       </c>
       <c r="E278" t="n">
-        <v>475</v>
+        <v>435</v>
       </c>
       <c r="F278" t="n">
-        <v>12.5</v>
+        <v>11</v>
       </c>
       <c r="G278" t="n">
-        <v>46</v>
+        <v>46.5</v>
       </c>
       <c r="H278" t="n">
         <v>19</v>
@@ -9631,10 +9631,10 @@
         </is>
       </c>
       <c r="D279" t="n">
-        <v>-190</v>
+        <v>-170</v>
       </c>
       <c r="E279" t="n">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F279" t="n">
         <v>3.5</v>
@@ -9646,6 +9646,237 @@
         <v>19</v>
       </c>
       <c r="I279" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>tennessee-titans</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>cincinnati-bengals</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>-200</v>
+      </c>
+      <c r="E280" t="n">
+        <v>170</v>
+      </c>
+      <c r="F280" t="n">
+        <v>4</v>
+      </c>
+      <c r="G280" t="n">
+        <v>48</v>
+      </c>
+      <c r="H280" t="n">
+        <v>20</v>
+      </c>
+      <c r="I280" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>green-bay-packers</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>san-francisco-49ers</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>-240</v>
+      </c>
+      <c r="E281" t="n">
+        <v>195</v>
+      </c>
+      <c r="F281" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="G281" t="n">
+        <v>47</v>
+      </c>
+      <c r="H281" t="n">
+        <v>20</v>
+      </c>
+      <c r="I281" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>tampa-bay-buccaneers</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>los-angeles-rams</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>-140</v>
+      </c>
+      <c r="E282" t="n">
+        <v>120</v>
+      </c>
+      <c r="F282" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G282" t="n">
+        <v>48</v>
+      </c>
+      <c r="H282" t="n">
+        <v>20</v>
+      </c>
+      <c r="I282" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>kansas-city-chiefs</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>buffalo-bills</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>-130</v>
+      </c>
+      <c r="E283" t="n">
+        <v>110</v>
+      </c>
+      <c r="F283" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G283" t="n">
+        <v>54</v>
+      </c>
+      <c r="H283" t="n">
+        <v>20</v>
+      </c>
+      <c r="I283" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>kansas-city-chiefs</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>cincinnati-bengals</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>-350</v>
+      </c>
+      <c r="E284" t="n">
+        <v>270</v>
+      </c>
+      <c r="F284" t="n">
+        <v>7</v>
+      </c>
+      <c r="G284" t="n">
+        <v>54.5</v>
+      </c>
+      <c r="H284" t="n">
+        <v>21</v>
+      </c>
+      <c r="I284" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>283</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>los-angeles-rams</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>san-francisco-49ers</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>-180</v>
+      </c>
+      <c r="E285" t="n">
+        <v>155</v>
+      </c>
+      <c r="F285" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G285" t="n">
+        <v>45.5</v>
+      </c>
+      <c r="H285" t="n">
+        <v>21</v>
+      </c>
+      <c r="I285" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>cincinnati-bengals</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>los-angeles-rams</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>170</v>
+      </c>
+      <c r="E286" t="n">
+        <v>-200</v>
+      </c>
+      <c r="F286" t="n">
+        <v>4</v>
+      </c>
+      <c r="G286" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="H286" t="n">
+        <v>22</v>
+      </c>
+      <c r="I286" t="n">
         <v>2021</v>
       </c>
     </row>

</xml_diff>